<commit_message>
[master] finished php tutorial_06
</commit_message>
<xml_diff>
--- a/tutorials/review_points_WaiLinOo .xlsx
+++ b/tutorials/review_points_WaiLinOo .xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="43">
   <si>
     <t>№</t>
   </si>
@@ -114,13 +114,25 @@
     <t>1) Use an indent of 4 spaces for *.php</t>
   </si>
   <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>Tutorial_05 index.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) is ok but test with more data in sample files </t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>12/20/2021 12:19PM</t>
+  </si>
+  <si>
     <t>エラータイプ</t>
   </si>
   <si>
     <t>Design</t>
-  </si>
-  <si>
-    <t>Unknown</t>
   </si>
   <si>
     <t>Request</t>
@@ -149,9 +161,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="22">
@@ -169,6 +181,36 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -183,31 +225,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -221,9 +249,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -260,6 +295,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -268,38 +310,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -313,7 +325,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -346,19 +358,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -370,145 +514,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -654,6 +666,32 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -679,6 +717,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -695,11 +748,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -712,192 +763,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="18" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1986,8 +1998,8 @@
   <sheetPr/>
   <dimension ref="A1:X7"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="92" zoomScaleNormal="100" topLeftCell="J3" workbookViewId="0">
-      <selection activeCell="X5" sqref="X5"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="92" zoomScaleNormal="100" topLeftCell="J4" workbookViewId="0">
+      <selection activeCell="W6" sqref="W6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12" outlineLevelRow="6"/>
@@ -2247,29 +2259,51 @@
       <c r="X5" s="28"/>
     </row>
     <row r="6" ht="135" customHeight="1" spans="1:24">
-      <c r="A6" s="9"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="13"/>
+      <c r="A6" s="9">
+        <v>5</v>
+      </c>
+      <c r="B6" s="10">
+        <v>44550</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>30</v>
+      </c>
       <c r="G6" s="14"/>
       <c r="H6" s="15"/>
-      <c r="I6" s="13"/>
+      <c r="I6" s="13" t="s">
+        <v>31</v>
+      </c>
       <c r="J6" s="14"/>
       <c r="K6" s="14"/>
       <c r="L6" s="14"/>
       <c r="M6" s="14"/>
       <c r="N6" s="15"/>
-      <c r="O6" s="20"/>
-      <c r="P6" s="24"/>
+      <c r="O6" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="P6" s="24" t="s">
+        <v>32</v>
+      </c>
       <c r="Q6" s="29"/>
       <c r="R6" s="29"/>
       <c r="S6" s="29"/>
       <c r="T6" s="29"/>
       <c r="U6" s="30"/>
-      <c r="V6" s="28"/>
-      <c r="W6" s="28"/>
+      <c r="V6" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="W6" s="28" t="s">
+        <v>19</v>
+      </c>
       <c r="X6" s="28"/>
     </row>
     <row r="7" ht="198.6" customHeight="1" spans="1:24">
@@ -2372,7 +2406,7 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>7</v>
@@ -2386,10 +2420,10 @@
         <v>12</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>17</v>
@@ -2400,10 +2434,10 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>14</v>
@@ -2413,13 +2447,13 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -2428,7 +2462,7 @@
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -2437,7 +2471,7 @@
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -2446,7 +2480,7 @@
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>

</xml_diff>

<commit_message>
[master]finished php tutorial6 and review update
</commit_message>
<xml_diff>
--- a/tutorials/review_points_WaiLinOo .xlsx
+++ b/tutorials/review_points_WaiLinOo .xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="42">
   <si>
     <t>№</t>
   </si>
@@ -121,9 +121,6 @@
   </si>
   <si>
     <t xml:space="preserve">1) is ok but test with more data in sample files </t>
-  </si>
-  <si>
-    <t>Done</t>
   </si>
   <si>
     <t>12/20/2021 12:19PM</t>
@@ -161,10 +158,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -181,20 +178,26 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -210,16 +213,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -234,33 +245,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -295,13 +283,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -317,19 +298,35 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -358,169 +355,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -668,11 +665,24 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -717,21 +727,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -749,17 +744,19 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -768,148 +765,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="18" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="18" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1998,8 +1995,8 @@
   <sheetPr/>
   <dimension ref="A1:X7"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="92" zoomScaleNormal="100" topLeftCell="J4" workbookViewId="0">
-      <selection activeCell="W6" sqref="W6"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="92" zoomScaleNormal="100" topLeftCell="J5" workbookViewId="0">
+      <selection activeCell="V6" sqref="V6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12" outlineLevelRow="6"/>
@@ -2291,7 +2288,7 @@
         <v>17</v>
       </c>
       <c r="P6" s="24" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="Q6" s="29"/>
       <c r="R6" s="29"/>
@@ -2299,7 +2296,7 @@
       <c r="T6" s="29"/>
       <c r="U6" s="30"/>
       <c r="V6" s="28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="W6" s="28" t="s">
         <v>19</v>
@@ -2406,7 +2403,7 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>7</v>
@@ -2420,7 +2417,7 @@
         <v>12</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>29</v>
@@ -2434,10 +2431,10 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>37</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>14</v>
@@ -2447,13 +2444,13 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -2462,7 +2459,7 @@
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -2471,7 +2468,7 @@
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -2480,7 +2477,7 @@
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>

</xml_diff>

<commit_message>
[master]finished php tutorial_7 and review update
</commit_message>
<xml_diff>
--- a/tutorials/review_points_WaiLinOo .xlsx
+++ b/tutorials/review_points_WaiLinOo .xlsx
@@ -135,7 +135,7 @@
     <t>1) Create folder under tutorial_06 (now in _actions folder)
 2) Not upload image when folder name is null
 3) Not create folder when image file is null
-4) Please return error message for input file is not image type</t>
+4) Please return error message for input file is not image type...</t>
   </si>
   <si>
     <t>Done error</t>
@@ -174,9 +174,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -192,8 +192,16 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -201,7 +209,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -215,13 +223,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -229,16 +230,15 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -247,6 +247,14 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -267,14 +275,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -291,22 +291,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -327,6 +321,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -335,9 +336,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -370,13 +370,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -388,151 +508,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -678,6 +678,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -741,15 +752,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -767,11 +769,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -780,148 +780,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2010,8 +2010,8 @@
   <sheetPr/>
   <dimension ref="A1:X7"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="92" zoomScaleNormal="100" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="92" zoomScaleNormal="100" topLeftCell="I6" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12" outlineLevelRow="6"/>

</xml_diff>